<commit_message>
corrected error in data download file
</commit_message>
<xml_diff>
--- a/data/download/financial-health-of-residents-data.xlsx
+++ b/data/download/financial-health-of-residents-data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EForney\Documents\00 DROP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/jpmc-60-cities/data/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="30645" windowHeight="20505" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="30640" windowHeight="20500"/>
   </bookViews>
   <sheets>
     <sheet name="City data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'City data'!$4:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -364,7 +364,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -499,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,11 +676,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1004,40 +1006,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B66" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="0.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="0.5" customWidth="1"/>
+    <col min="6" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="8" max="8" width="0.5" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
     <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" customWidth="1"/>
-    <col min="15" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="16" width="12.1640625" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" customWidth="1"/>
+    <col min="18" max="18" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>91</v>
       </c>
@@ -1059,7 +1061,7 @@
       <c r="Q1" s="63"/>
       <c r="R1" s="63"/>
     </row>
-    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>80</v>
       </c>
@@ -1085,39 +1087,39 @@
       <c r="U2" s="31"/>
       <c r="V2" s="31"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="M3" s="54"/>
       <c r="N3" s="54"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="67"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="69"/>
+      <c r="J4" s="71"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-    </row>
-    <row r="5" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+    </row>
+    <row r="5" spans="1:22" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1169,8 +1171,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A6" s="65" t="s">
+    <row r="6" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="67" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="65"/>
@@ -1191,18 +1193,18 @@
       <c r="Q6" s="65"/>
       <c r="R6" s="65"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B7" s="11">
         <v>720</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="11">
         <v>722</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13">
@@ -1244,7 +1246,7 @@
       </c>
       <c r="T7" s="55"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>56</v>
       </c>
@@ -1252,10 +1254,10 @@
         <v>732</v>
       </c>
       <c r="C8" s="11">
+        <v>746</v>
+      </c>
+      <c r="D8" s="11">
         <v>714</v>
-      </c>
-      <c r="D8" s="11">
-        <v>746</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13">
@@ -1296,7 +1298,7 @@
         <v>0.52079999446868896</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>57</v>
       </c>
@@ -1304,10 +1306,10 @@
         <v>714</v>
       </c>
       <c r="C9" s="11">
+        <v>746</v>
+      </c>
+      <c r="D9" s="11">
         <v>693</v>
-      </c>
-      <c r="D9" s="11">
-        <v>746</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="13">
@@ -1348,7 +1350,7 @@
         <v>0.45390000939369202</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>58</v>
       </c>
@@ -1356,10 +1358,10 @@
         <v>731</v>
       </c>
       <c r="C10" s="11">
+        <v>734</v>
+      </c>
+      <c r="D10" s="11">
         <v>668</v>
-      </c>
-      <c r="D10" s="11">
-        <v>734</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="13">
@@ -1400,8 +1402,8 @@
         <v>0.47569999098777771</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="66" t="s">
+    <row r="11" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="68" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="66"/>
@@ -1423,7 +1425,7 @@
       <c r="R11" s="66"/>
       <c r="T11" s="55"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" s="17" t="s">
         <v>39</v>
       </c>
@@ -1431,10 +1433,10 @@
         <v>667</v>
       </c>
       <c r="C12" s="18">
+        <v>732</v>
+      </c>
+      <c r="D12" s="18">
         <v>626</v>
-      </c>
-      <c r="D12" s="18">
-        <v>732</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="20">
@@ -1475,7 +1477,7 @@
         <v>0.47780001163482666</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="17" t="s">
         <v>52</v>
       </c>
@@ -1483,10 +1485,10 @@
         <v>716</v>
       </c>
       <c r="C13" s="18">
+        <v>723</v>
+      </c>
+      <c r="D13" s="18">
         <v>632</v>
-      </c>
-      <c r="D13" s="18">
-        <v>723</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="20">
@@ -1527,7 +1529,7 @@
         <v>0.54549998044967651</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="17" t="s">
         <v>53</v>
       </c>
@@ -1535,10 +1537,10 @@
         <v>663</v>
       </c>
       <c r="C14" s="18">
+        <v>714</v>
+      </c>
+      <c r="D14" s="18">
         <v>633</v>
-      </c>
-      <c r="D14" s="18">
-        <v>714</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="20">
@@ -1579,7 +1581,7 @@
         <v>0.53049999475479126</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" s="17" t="s">
         <v>46</v>
       </c>
@@ -1587,10 +1589,10 @@
         <v>701</v>
       </c>
       <c r="C15" s="18">
+        <v>728</v>
+      </c>
+      <c r="D15" s="18">
         <v>570</v>
-      </c>
-      <c r="D15" s="18">
-        <v>728</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="20">
@@ -1631,7 +1633,7 @@
         <v>0.50639998912811279</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" s="17" t="s">
         <v>54</v>
       </c>
@@ -1639,10 +1641,10 @@
         <v>708</v>
       </c>
       <c r="C16" s="18">
+        <v>740</v>
+      </c>
+      <c r="D16" s="18">
         <v>648</v>
-      </c>
-      <c r="D16" s="18">
-        <v>740</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20">
@@ -1683,7 +1685,7 @@
         <v>0.55140000581741333</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="17" t="s">
         <v>55</v>
       </c>
@@ -1691,10 +1693,10 @@
         <v>668</v>
       </c>
       <c r="C17" s="18">
+        <v>759.5</v>
+      </c>
+      <c r="D17" s="18">
         <v>624</v>
-      </c>
-      <c r="D17" s="18">
-        <v>759.5</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20">
@@ -1735,7 +1737,7 @@
         <v>0.50690001249313354</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" s="17" t="s">
         <v>50</v>
       </c>
@@ -1743,10 +1745,10 @@
         <v>689</v>
       </c>
       <c r="C18" s="18">
+        <v>720</v>
+      </c>
+      <c r="D18" s="18">
         <v>586</v>
-      </c>
-      <c r="D18" s="18">
-        <v>720</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20">
@@ -1787,18 +1789,18 @@
         <v>0.47960001230239868</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B19" s="18">
         <v>709</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="18">
+        <v>718</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="D19" s="18">
-        <v>718</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="20">
@@ -1839,7 +1841,7 @@
         <v>0.47679999470710754</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20" s="17" t="s">
         <v>40</v>
       </c>
@@ -1847,10 +1849,10 @@
         <v>662</v>
       </c>
       <c r="C20" s="18">
+        <v>679</v>
+      </c>
+      <c r="D20" s="18">
         <v>644</v>
-      </c>
-      <c r="D20" s="18">
-        <v>679</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="20">
@@ -1891,7 +1893,7 @@
         <v>0.46880000829696655</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>51</v>
       </c>
@@ -1899,10 +1901,10 @@
         <v>671</v>
       </c>
       <c r="C21" s="18">
+        <v>739</v>
+      </c>
+      <c r="D21" s="18">
         <v>617.5</v>
-      </c>
-      <c r="D21" s="18">
-        <v>739</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="20">
@@ -1948,8 +1950,8 @@
       <c r="V21" s="53"/>
       <c r="W21" s="54"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A22" s="65" t="s">
+    <row r="22" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="67" t="s">
         <v>84</v>
       </c>
       <c r="B22" s="65"/>
@@ -1970,7 +1972,7 @@
       <c r="Q22" s="65"/>
       <c r="R22" s="65"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
@@ -1978,10 +1980,10 @@
         <v>647</v>
       </c>
       <c r="C23" s="11">
+        <v>668</v>
+      </c>
+      <c r="D23" s="11">
         <v>560.5</v>
-      </c>
-      <c r="D23" s="11">
-        <v>668</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="13">
@@ -2022,7 +2024,7 @@
         <v>0.44209998846054077</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>44</v>
       </c>
@@ -2030,10 +2032,10 @@
         <v>670</v>
       </c>
       <c r="C24" s="11">
+        <v>675</v>
+      </c>
+      <c r="D24" s="11">
         <v>552</v>
-      </c>
-      <c r="D24" s="11">
-        <v>675</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="13">
@@ -2074,7 +2076,7 @@
         <v>0.46919998526573181</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
         <v>7</v>
       </c>
@@ -2082,10 +2084,10 @@
         <v>617</v>
       </c>
       <c r="C25" s="11">
+        <v>655</v>
+      </c>
+      <c r="D25" s="11">
         <v>566</v>
-      </c>
-      <c r="D25" s="11">
-        <v>655</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="13">
@@ -2126,7 +2128,7 @@
         <v>0.48170000314712524</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A26" s="10" t="s">
         <v>49</v>
       </c>
@@ -2134,10 +2136,10 @@
         <v>660</v>
       </c>
       <c r="C26" s="11">
+        <v>699</v>
+      </c>
+      <c r="D26" s="11">
         <v>552</v>
-      </c>
-      <c r="D26" s="11">
-        <v>699</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="13">
@@ -2178,18 +2180,18 @@
         <v>0.4749000072479248</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="11">
         <v>646</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="11">
+        <v>645</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="D27" s="11">
-        <v>645</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="13">
@@ -2212,7 +2214,7 @@
         <v>0.8760073184967041</v>
       </c>
       <c r="M27" s="13">
-        <v>0.35480117797851563</v>
+        <v>0.35480117797851562</v>
       </c>
       <c r="N27" s="15">
         <v>8.2825027406215668E-2</v>
@@ -2230,7 +2232,7 @@
         <v>0.45010000467300415</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A28" s="10" t="s">
         <v>45</v>
       </c>
@@ -2238,10 +2240,10 @@
         <v>668</v>
       </c>
       <c r="C28" s="11">
+        <v>690</v>
+      </c>
+      <c r="D28" s="11">
         <v>544</v>
-      </c>
-      <c r="D28" s="11">
-        <v>690</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="13">
@@ -2282,7 +2284,7 @@
         <v>0.47620001435279846</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A29" s="10" t="s">
         <v>2</v>
       </c>
@@ -2290,10 +2292,10 @@
         <v>627</v>
       </c>
       <c r="C29" s="11">
+        <v>699</v>
+      </c>
+      <c r="D29" s="11">
         <v>567</v>
-      </c>
-      <c r="D29" s="11">
-        <v>699</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="13">
@@ -2334,8 +2336,8 @@
         <v>0.47189998626708984</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="66" t="s">
+    <row r="30" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B30" s="66"/>
@@ -2357,7 +2359,7 @@
       <c r="R30" s="66"/>
       <c r="T30" s="55"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A31" s="24" t="s">
         <v>19</v>
       </c>
@@ -2365,10 +2367,10 @@
         <v>650</v>
       </c>
       <c r="C31" s="25">
+        <v>727</v>
+      </c>
+      <c r="D31" s="25">
         <v>560</v>
-      </c>
-      <c r="D31" s="25">
-        <v>727</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="27">
@@ -2409,7 +2411,7 @@
         <v>0.57120001316070557</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A32" s="24" t="s">
         <v>21</v>
       </c>
@@ -2417,10 +2419,10 @@
         <v>654.5</v>
       </c>
       <c r="C32" s="25">
+        <v>693</v>
+      </c>
+      <c r="D32" s="25">
         <v>563</v>
-      </c>
-      <c r="D32" s="25">
-        <v>693</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="27">
@@ -2461,7 +2463,7 @@
         <v>0.50180000066757202</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" s="24" t="s">
         <v>20</v>
       </c>
@@ -2469,10 +2471,10 @@
         <v>656</v>
       </c>
       <c r="C33" s="25">
+        <v>732</v>
+      </c>
+      <c r="D33" s="25">
         <v>586</v>
-      </c>
-      <c r="D33" s="25">
-        <v>732</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="27">
@@ -2513,7 +2515,7 @@
         <v>0.53140002489089966</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" s="24" t="s">
         <v>25</v>
       </c>
@@ -2521,10 +2523,10 @@
         <v>672</v>
       </c>
       <c r="C34" s="25">
+        <v>693</v>
+      </c>
+      <c r="D34" s="25">
         <v>572</v>
-      </c>
-      <c r="D34" s="25">
-        <v>693</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34" s="27">
@@ -2565,7 +2567,7 @@
         <v>0.54070001840591431</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" s="24" t="s">
         <v>22</v>
       </c>
@@ -2573,10 +2575,10 @@
         <v>707</v>
       </c>
       <c r="C35" s="25">
+        <v>720</v>
+      </c>
+      <c r="D35" s="25">
         <v>590.5</v>
-      </c>
-      <c r="D35" s="25">
-        <v>720</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="27">
@@ -2617,7 +2619,7 @@
         <v>0.53880000114440918</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" s="24" t="s">
         <v>23</v>
       </c>
@@ -2625,10 +2627,10 @@
         <v>665</v>
       </c>
       <c r="C36" s="25">
+        <v>732</v>
+      </c>
+      <c r="D36" s="25">
         <v>552</v>
-      </c>
-      <c r="D36" s="25">
-        <v>732</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="27">
@@ -2669,7 +2671,7 @@
         <v>0.50989997386932373</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37" s="24" t="s">
         <v>24</v>
       </c>
@@ -2677,10 +2679,10 @@
         <v>675</v>
       </c>
       <c r="C37" s="25">
+        <v>722</v>
+      </c>
+      <c r="D37" s="25">
         <v>554</v>
-      </c>
-      <c r="D37" s="25">
-        <v>722</v>
       </c>
       <c r="E37" s="26"/>
       <c r="F37" s="27">
@@ -2722,8 +2724,8 @@
       </c>
       <c r="T37" s="55"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="65" t="s">
+    <row r="38" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="67" t="s">
         <v>86</v>
       </c>
       <c r="B38" s="65"/>
@@ -2744,7 +2746,7 @@
       <c r="Q38" s="65"/>
       <c r="R38" s="65"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="10" t="s">
         <v>35</v>
       </c>
@@ -2752,10 +2754,10 @@
         <v>675</v>
       </c>
       <c r="C39" s="11">
+        <v>732</v>
+      </c>
+      <c r="D39" s="11">
         <v>582</v>
-      </c>
-      <c r="D39" s="11">
-        <v>732</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="13">
@@ -2796,7 +2798,7 @@
         <v>0.48719999194145203</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="10" t="s">
         <v>38</v>
       </c>
@@ -2804,10 +2806,10 @@
         <v>654</v>
       </c>
       <c r="C40" s="11">
+        <v>723.5</v>
+      </c>
+      <c r="D40" s="11">
         <v>598</v>
-      </c>
-      <c r="D40" s="11">
-        <v>723.5</v>
       </c>
       <c r="E40" s="12"/>
       <c r="F40" s="13">
@@ -2848,7 +2850,7 @@
         <v>0.49639999866485596</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
         <v>43</v>
       </c>
@@ -2856,10 +2858,10 @@
         <v>675</v>
       </c>
       <c r="C41" s="11">
+        <v>714.5</v>
+      </c>
+      <c r="D41" s="11">
         <v>605</v>
-      </c>
-      <c r="D41" s="11">
-        <v>714.5</v>
       </c>
       <c r="E41" s="12"/>
       <c r="F41" s="13">
@@ -2900,7 +2902,7 @@
         <v>0.4927000105381012</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="10" t="s">
         <v>42</v>
       </c>
@@ -2908,10 +2910,10 @@
         <v>666</v>
       </c>
       <c r="C42" s="11">
+        <v>715.5</v>
+      </c>
+      <c r="D42" s="11">
         <v>602</v>
-      </c>
-      <c r="D42" s="11">
-        <v>715.5</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="13">
@@ -2952,7 +2954,7 @@
         <v>0.47209998965263367</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
         <v>36</v>
       </c>
@@ -2960,10 +2962,10 @@
         <v>665</v>
       </c>
       <c r="C43" s="11">
+        <v>706</v>
+      </c>
+      <c r="D43" s="11">
         <v>559</v>
-      </c>
-      <c r="D43" s="11">
-        <v>706</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="13">
@@ -3004,7 +3006,7 @@
         <v>0.47350001335144043</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44" s="40" t="s">
         <v>37</v>
       </c>
@@ -3012,10 +3014,10 @@
         <v>642</v>
       </c>
       <c r="C44" s="41">
+        <v>676</v>
+      </c>
+      <c r="D44" s="41">
         <v>590</v>
-      </c>
-      <c r="D44" s="41">
-        <v>676</v>
       </c>
       <c r="E44" s="42"/>
       <c r="F44" s="43">
@@ -3057,8 +3059,8 @@
       </c>
       <c r="U44" s="53"/>
     </row>
-    <row r="45" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="66" t="s">
+    <row r="45" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="68" t="s">
         <v>87</v>
       </c>
       <c r="B45" s="66"/>
@@ -3080,7 +3082,7 @@
       <c r="R45" s="66"/>
       <c r="T45" s="55"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="24" t="s">
         <v>28</v>
       </c>
@@ -3088,10 +3090,10 @@
         <v>626</v>
       </c>
       <c r="C46" s="25">
+        <v>717</v>
+      </c>
+      <c r="D46" s="25">
         <v>561</v>
-      </c>
-      <c r="D46" s="25">
-        <v>717</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="27">
@@ -3132,7 +3134,7 @@
         <v>0.54869997501373291</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="24" t="s">
         <v>27</v>
       </c>
@@ -3140,10 +3142,10 @@
         <v>642</v>
       </c>
       <c r="C47" s="25">
+        <v>735</v>
+      </c>
+      <c r="D47" s="25">
         <v>600</v>
-      </c>
-      <c r="D47" s="25">
-        <v>735</v>
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="27">
@@ -3184,7 +3186,7 @@
         <v>0.52859997749328613</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48" s="24" t="s">
         <v>33</v>
       </c>
@@ -3192,10 +3194,10 @@
         <v>644</v>
       </c>
       <c r="C48" s="25">
+        <v>702</v>
+      </c>
+      <c r="D48" s="25">
         <v>573</v>
-      </c>
-      <c r="D48" s="25">
-        <v>702</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="27">
@@ -3236,7 +3238,7 @@
         <v>0.47440001368522644</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A49" s="24" t="s">
         <v>26</v>
       </c>
@@ -3244,10 +3246,10 @@
         <v>638</v>
       </c>
       <c r="C49" s="25">
+        <v>697</v>
+      </c>
+      <c r="D49" s="25">
         <v>560</v>
-      </c>
-      <c r="D49" s="25">
-        <v>697</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="27">
@@ -3288,18 +3290,18 @@
         <v>0.53930002450942993</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A50" s="24" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="25">
         <v>660</v>
       </c>
-      <c r="C50" s="25">
+      <c r="C50" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="25">
         <v>652</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>93</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="27">
@@ -3340,7 +3342,7 @@
         <v>0.57620000839233398</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A51" s="24" t="s">
         <v>41</v>
       </c>
@@ -3348,10 +3350,10 @@
         <v>644</v>
       </c>
       <c r="C51" s="25">
+        <v>677</v>
+      </c>
+      <c r="D51" s="25">
         <v>566</v>
-      </c>
-      <c r="D51" s="25">
-        <v>677</v>
       </c>
       <c r="E51" s="26"/>
       <c r="F51" s="27">
@@ -3392,7 +3394,7 @@
         <v>0.48930001258850098</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A52" s="24" t="s">
         <v>34</v>
       </c>
@@ -3400,10 +3402,10 @@
         <v>646</v>
       </c>
       <c r="C52" s="25">
+        <v>721</v>
+      </c>
+      <c r="D52" s="25">
         <v>615</v>
-      </c>
-      <c r="D52" s="25">
-        <v>721</v>
       </c>
       <c r="E52" s="26"/>
       <c r="F52" s="27">
@@ -3444,7 +3446,7 @@
         <v>0.46309998631477356</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A53" s="24" t="s">
         <v>29</v>
       </c>
@@ -3452,10 +3454,10 @@
         <v>640</v>
       </c>
       <c r="C53" s="25">
+        <v>677</v>
+      </c>
+      <c r="D53" s="25">
         <v>552</v>
-      </c>
-      <c r="D53" s="25">
-        <v>677</v>
       </c>
       <c r="E53" s="26"/>
       <c r="F53" s="27">
@@ -3497,8 +3499,8 @@
       </c>
       <c r="T53" s="55"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A54" s="65" t="s">
+    <row r="54" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="67" t="s">
         <v>88</v>
       </c>
       <c r="B54" s="65"/>
@@ -3519,7 +3521,7 @@
       <c r="Q54" s="65"/>
       <c r="R54" s="65"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A55" s="10" t="s">
         <v>8</v>
       </c>
@@ -3527,10 +3529,10 @@
         <v>623</v>
       </c>
       <c r="C55" s="11">
+        <v>671</v>
+      </c>
+      <c r="D55" s="11">
         <v>576</v>
-      </c>
-      <c r="D55" s="11">
-        <v>671</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="13">
@@ -3571,7 +3573,7 @@
         <v>0.51920002698898315</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A56" s="10" t="s">
         <v>0</v>
       </c>
@@ -3579,10 +3581,10 @@
         <v>633</v>
       </c>
       <c r="C56" s="11">
+        <v>708.5</v>
+      </c>
+      <c r="D56" s="11">
         <v>587</v>
-      </c>
-      <c r="D56" s="11">
-        <v>708.5</v>
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="13">
@@ -3623,18 +3625,18 @@
         <v>0.47769999504089355</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A57" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="11">
         <v>593</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="11">
         <v>581</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="13">
@@ -3675,7 +3677,7 @@
         <v>0.45030000805854797</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A58" s="10" t="s">
         <v>6</v>
       </c>
@@ -3683,10 +3685,10 @@
         <v>628</v>
       </c>
       <c r="C58" s="11">
+        <v>703</v>
+      </c>
+      <c r="D58" s="11">
         <v>571</v>
-      </c>
-      <c r="D58" s="11">
-        <v>703</v>
       </c>
       <c r="E58" s="12"/>
       <c r="F58" s="13">
@@ -3727,7 +3729,7 @@
         <v>0.50489997863769531</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A59" s="10" t="s">
         <v>4</v>
       </c>
@@ -3735,10 +3737,10 @@
         <v>675</v>
       </c>
       <c r="C59" s="11">
+        <v>723</v>
+      </c>
+      <c r="D59" s="11">
         <v>552</v>
-      </c>
-      <c r="D59" s="11">
-        <v>723</v>
       </c>
       <c r="E59" s="12"/>
       <c r="F59" s="13">
@@ -3779,18 +3781,18 @@
         <v>0.46570000052452087</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A60" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B60" s="11">
         <v>588.5</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="11">
         <v>586</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="E60" s="12"/>
       <c r="F60" s="13">
@@ -3833,8 +3835,8 @@
       <c r="S60" s="54"/>
       <c r="T60" s="55"/>
     </row>
-    <row r="61" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="66" t="s">
+    <row r="61" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="68" t="s">
         <v>89</v>
       </c>
       <c r="B61" s="66"/>
@@ -3856,7 +3858,7 @@
       <c r="R61" s="66"/>
       <c r="T61" s="55"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A62" s="24" t="s">
         <v>15</v>
       </c>
@@ -3864,10 +3866,10 @@
         <v>649</v>
       </c>
       <c r="C62" s="25">
+        <v>703</v>
+      </c>
+      <c r="D62" s="25">
         <v>567</v>
-      </c>
-      <c r="D62" s="25">
-        <v>703</v>
       </c>
       <c r="E62" s="26"/>
       <c r="F62" s="27">
@@ -3908,7 +3910,7 @@
         <v>0.50489997863769531</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A63" s="24" t="s">
         <v>17</v>
       </c>
@@ -3916,10 +3918,10 @@
         <v>597</v>
       </c>
       <c r="C63" s="25">
+        <v>697</v>
+      </c>
+      <c r="D63" s="25">
         <v>552</v>
-      </c>
-      <c r="D63" s="25">
-        <v>697</v>
       </c>
       <c r="E63" s="26"/>
       <c r="F63" s="27">
@@ -3960,7 +3962,7 @@
         <v>0.48260000348091125</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A64" s="24" t="s">
         <v>18</v>
       </c>
@@ -3968,10 +3970,10 @@
         <v>626</v>
       </c>
       <c r="C64" s="25">
+        <v>676</v>
+      </c>
+      <c r="D64" s="25">
         <v>552</v>
-      </c>
-      <c r="D64" s="25">
-        <v>676</v>
       </c>
       <c r="E64" s="26"/>
       <c r="F64" s="27">
@@ -4012,7 +4014,7 @@
         <v>0.48910000920295715</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A65" s="24" t="s">
         <v>14</v>
       </c>
@@ -4020,10 +4022,10 @@
         <v>640</v>
       </c>
       <c r="C65" s="25">
+        <v>675</v>
+      </c>
+      <c r="D65" s="25">
         <v>602</v>
-      </c>
-      <c r="D65" s="25">
-        <v>675</v>
       </c>
       <c r="E65" s="26"/>
       <c r="F65" s="27">
@@ -4064,7 +4066,7 @@
         <v>0.51649999618530273</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A66" s="24" t="s">
         <v>9</v>
       </c>
@@ -4072,10 +4074,10 @@
         <v>619</v>
       </c>
       <c r="C66" s="25">
+        <v>661</v>
+      </c>
+      <c r="D66" s="25">
         <v>581</v>
-      </c>
-      <c r="D66" s="25">
-        <v>661</v>
       </c>
       <c r="E66" s="26"/>
       <c r="F66" s="27">
@@ -4116,7 +4118,7 @@
         <v>0.49700000882148743</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A67" s="24" t="s">
         <v>10</v>
       </c>
@@ -4124,10 +4126,10 @@
         <v>586</v>
       </c>
       <c r="C67" s="25">
+        <v>648</v>
+      </c>
+      <c r="D67" s="25">
         <v>557</v>
-      </c>
-      <c r="D67" s="25">
-        <v>648</v>
       </c>
       <c r="E67" s="26"/>
       <c r="F67" s="27">
@@ -4168,7 +4170,7 @@
         <v>0.5031999945640564</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A68" s="24" t="s">
         <v>16</v>
       </c>
@@ -4176,10 +4178,10 @@
         <v>618</v>
       </c>
       <c r="C68" s="25">
+        <v>683</v>
+      </c>
+      <c r="D68" s="25">
         <v>586</v>
-      </c>
-      <c r="D68" s="25">
-        <v>683</v>
       </c>
       <c r="E68" s="26"/>
       <c r="F68" s="27">
@@ -4220,7 +4222,7 @@
         <v>0.50880002975463867</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A69" s="24" t="s">
         <v>12</v>
       </c>
@@ -4228,10 +4230,10 @@
         <v>629</v>
       </c>
       <c r="C69" s="25">
+        <v>707</v>
+      </c>
+      <c r="D69" s="25">
         <v>586</v>
-      </c>
-      <c r="D69" s="25">
-        <v>707</v>
       </c>
       <c r="E69" s="26"/>
       <c r="F69" s="27">
@@ -4272,7 +4274,7 @@
         <v>0.56360000371932983</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A70" s="24" t="s">
         <v>11</v>
       </c>
@@ -4280,10 +4282,10 @@
         <v>624</v>
       </c>
       <c r="C70" s="25">
+        <v>735</v>
+      </c>
+      <c r="D70" s="25">
         <v>552</v>
-      </c>
-      <c r="D70" s="25">
-        <v>735</v>
       </c>
       <c r="E70" s="26"/>
       <c r="F70" s="27">
@@ -4324,7 +4326,7 @@
         <v>0.49790000915527344</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A71" s="24" t="s">
         <v>13</v>
       </c>
@@ -4332,10 +4334,10 @@
         <v>601</v>
       </c>
       <c r="C71" s="25">
+        <v>672.5</v>
+      </c>
+      <c r="D71" s="25">
         <v>552</v>
-      </c>
-      <c r="D71" s="25">
-        <v>672.5</v>
       </c>
       <c r="E71" s="26"/>
       <c r="F71" s="27">
@@ -4376,8 +4378,8 @@
         <v>0.506600022315979</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="65" t="s">
+    <row r="72" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="67" t="s">
         <v>90</v>
       </c>
       <c r="B72" s="65"/>
@@ -4398,7 +4400,7 @@
       <c r="Q72" s="65"/>
       <c r="R72" s="65"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A73" s="10" t="s">
         <v>31</v>
       </c>
@@ -4406,10 +4408,10 @@
         <v>552</v>
       </c>
       <c r="C73" s="11">
+        <v>615</v>
+      </c>
+      <c r="D73" s="11">
         <v>552</v>
-      </c>
-      <c r="D73" s="11">
-        <v>615</v>
       </c>
       <c r="E73" s="12"/>
       <c r="F73" s="13">
@@ -4450,18 +4452,18 @@
         <v>0.51719999313354492</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A74" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B74" s="11">
         <v>570</v>
       </c>
-      <c r="C74" s="11">
+      <c r="C74" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="11">
         <v>567</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="E74" s="12"/>
       <c r="F74" s="13">
@@ -4502,7 +4504,7 @@
         <v>0.50279998779296875</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="60" t="s">
         <v>101</v>
       </c>
@@ -4512,11 +4514,11 @@
       </c>
       <c r="C75" s="47">
         <f>AVERAGE(C7:C44,C46:C74)</f>
-        <v>589.14655172413791</v>
+        <v>703.63636363636363</v>
       </c>
       <c r="D75" s="47">
         <f>AVERAGE(D7:D44,D46:D74)</f>
-        <v>703.63636363636363</v>
+        <v>589.14655172413791</v>
       </c>
       <c r="E75" s="48" t="e">
         <v>#DIV/0!</v>
@@ -4573,7 +4575,7 @@
         <v>0.4999666675925255</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A76" s="59" t="s">
         <v>102</v>
       </c>
@@ -4581,10 +4583,10 @@
         <v>675</v>
       </c>
       <c r="C76" s="33">
+        <v>697</v>
+      </c>
+      <c r="D76" s="33">
         <v>621</v>
-      </c>
-      <c r="D76" s="33">
-        <v>697</v>
       </c>
       <c r="E76" s="33"/>
       <c r="F76" s="34">
@@ -4625,52 +4627,43 @@
         <v>0.48170000314712524</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A77" s="39" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A78" s="39" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A79" s="39" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A80" s="39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A81" s="39" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A82" s="39"/>
     </row>
   </sheetData>
   <sortState ref="A7:R74">
     <sortCondition ref="A7:A74"/>
   </sortState>
-  <mergeCells count="13">
-    <mergeCell ref="A72:R72"/>
-    <mergeCell ref="A30:R30"/>
-    <mergeCell ref="A45:R45"/>
-    <mergeCell ref="A61:R61"/>
+  <mergeCells count="4">
     <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A6:R6"/>
-    <mergeCell ref="A11:R11"/>
-    <mergeCell ref="A22:R22"/>
-    <mergeCell ref="A38:R38"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A54:R54"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4684,38 +4677,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="0.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="0.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0.5" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="0.5" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
         <v>91</v>
       </c>
@@ -4737,40 +4730,40 @@
       <c r="Q1" s="63"/>
       <c r="R1" s="63"/>
     </row>
-    <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="56"/>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="67"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="69" t="s">
+      <c r="I4" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="J4" s="69"/>
+      <c r="J4" s="71"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-    </row>
-    <row r="5" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+    </row>
+    <row r="5" spans="1:18" ht="52" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
@@ -4822,7 +4815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="61" t="s">
         <v>82</v>
       </c>
@@ -4830,10 +4823,10 @@
         <v>724.25</v>
       </c>
       <c r="C6" s="11">
+        <v>742</v>
+      </c>
+      <c r="D6" s="11">
         <v>699.25</v>
-      </c>
-      <c r="D6" s="11">
-        <v>742</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="13">
@@ -4874,7 +4867,7 @@
         <v>0.4773</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="62" t="s">
         <v>83</v>
       </c>
@@ -4882,10 +4875,10 @@
         <v>685.4</v>
       </c>
       <c r="C7" s="25">
+        <v>725.25</v>
+      </c>
+      <c r="D7" s="25">
         <v>620.05555555555554</v>
-      </c>
-      <c r="D7" s="25">
-        <v>725.25</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="27">
@@ -4926,7 +4919,7 @@
         <v>0.50790000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="61" t="s">
         <v>84</v>
       </c>
@@ -4934,10 +4927,10 @@
         <v>647.85709999999995</v>
       </c>
       <c r="C8" s="11">
+        <v>675.85709999999995</v>
+      </c>
+      <c r="D8" s="11">
         <v>556.91669999999999</v>
-      </c>
-      <c r="D8" s="11">
-        <v>675.85709999999995</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="13">
@@ -4978,7 +4971,7 @@
         <v>0.46660000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="62" t="s">
         <v>85</v>
       </c>
@@ -4986,10 +4979,10 @@
         <v>668.5</v>
       </c>
       <c r="C9" s="25">
+        <v>717</v>
+      </c>
+      <c r="D9" s="25">
         <v>568.21429999999998</v>
-      </c>
-      <c r="D9" s="25">
-        <v>717</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="27">
@@ -5030,7 +5023,7 @@
         <v>0.53439999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="61" t="s">
         <v>86</v>
       </c>
@@ -5038,10 +5031,10 @@
         <v>662.83330000000001</v>
       </c>
       <c r="C10" s="11">
+        <v>711.25</v>
+      </c>
+      <c r="D10" s="11">
         <v>589.33330000000001</v>
-      </c>
-      <c r="D10" s="11">
-        <v>711.25</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="13">
@@ -5082,7 +5075,7 @@
         <v>0.48470000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="62" t="s">
         <v>87</v>
       </c>
@@ -5090,10 +5083,10 @@
         <v>642.5</v>
       </c>
       <c r="C11" s="25">
+        <v>704</v>
+      </c>
+      <c r="D11" s="25">
         <v>584.875</v>
-      </c>
-      <c r="D11" s="25">
-        <v>704</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="27">
@@ -5134,7 +5127,7 @@
         <v>0.51800000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A12" s="61" t="s">
         <v>88</v>
       </c>
@@ -5142,10 +5135,10 @@
         <v>623.41669999999999</v>
       </c>
       <c r="C12" s="11">
+        <v>701.375</v>
+      </c>
+      <c r="D12" s="11">
         <v>575.5</v>
-      </c>
-      <c r="D12" s="11">
-        <v>701.375</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="13">
@@ -5186,7 +5179,7 @@
         <v>0.47689999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A13" s="62" t="s">
         <v>89</v>
       </c>
@@ -5194,10 +5187,10 @@
         <v>618.9</v>
       </c>
       <c r="C13" s="25">
+        <v>685.75</v>
+      </c>
+      <c r="D13" s="25">
         <v>568.70000000000005</v>
-      </c>
-      <c r="D13" s="25">
-        <v>685.75</v>
       </c>
       <c r="E13" s="25"/>
       <c r="F13" s="27">
@@ -5238,7 +5231,7 @@
         <v>0.50700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" s="61" t="s">
         <v>90</v>
       </c>
@@ -5246,10 +5239,10 @@
         <v>561</v>
       </c>
       <c r="C14" s="11">
+        <v>615</v>
+      </c>
+      <c r="D14" s="11">
         <v>559.5</v>
-      </c>
-      <c r="D14" s="11">
-        <v>615</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="13">
@@ -5290,7 +5283,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="57" t="s">
         <v>101</v>
       </c>
@@ -5298,10 +5291,10 @@
         <v>652.23333333333335</v>
       </c>
       <c r="C15" s="47">
+        <v>703.63636363636363</v>
+      </c>
+      <c r="D15" s="47">
         <v>589.14655172413791</v>
-      </c>
-      <c r="D15" s="47">
-        <v>703.63636363636363</v>
       </c>
       <c r="E15" s="47"/>
       <c r="F15" s="49">
@@ -5342,7 +5335,7 @@
         <v>0.4999666675925255</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" s="58" t="s">
         <v>102</v>
       </c>
@@ -5350,10 +5343,10 @@
         <v>675</v>
       </c>
       <c r="C16" s="33">
+        <v>697</v>
+      </c>
+      <c r="D16" s="33">
         <v>621</v>
-      </c>
-      <c r="D16" s="33">
-        <v>697</v>
       </c>
       <c r="E16" s="33"/>
       <c r="F16" s="34">
@@ -5394,7 +5387,7 @@
         <v>0.48170000314712524</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="39" t="s">
         <v>96</v>
       </c>

</xml_diff>